<commit_message>
Some progress on capture protocol.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Capture_preparation_v3_14_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Capture_preparation_v3_14_0.xlsx
@@ -176,7 +176,7 @@
     <t xml:space="preserve">Container Kind</t>
   </si>
   <si>
-    <t xml:space="preserve">Capture-MCC</t>
+    <t xml:space="preserve">MCC</t>
   </si>
   <si>
     <t xml:space="preserve">Janick St-Cyr</t>
@@ -197,7 +197,7 @@
     <t xml:space="preserve">tube</t>
   </si>
   <si>
-    <t xml:space="preserve">Capture-Exome</t>
+    <t xml:space="preserve">Exome</t>
   </si>
   <si>
     <t xml:space="preserve">Elizabeth Caron</t>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">96-well plate</t>
   </si>
   <si>
-    <t xml:space="preserve">Capture-Panel</t>
+    <t xml:space="preserve">Panel</t>
   </si>
   <si>
     <t xml:space="preserve">Patrick Willett</t>
@@ -610,7 +610,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
@@ -8643,7 +8643,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.3"/>
@@ -17464,7 +17464,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>

</xml_diff>

<commit_message>
Merged capture library and convert library core function. Added migration for new protocol and library-selection.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Capture_preparation_v3_14_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Capture_preparation_v3_14_0.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
   <si>
     <t xml:space="preserve">Capture Preparation Template</t>
   </si>
@@ -610,7 +610,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
@@ -697,7 +697,9 @@
       <c r="G7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -8643,7 +8645,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.3"/>
@@ -17464,7 +17466,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>

</xml_diff>